<commit_message>
Hoàn thành chương 1, 2 Chương 3, 4 fake
</commit_message>
<xml_diff>
--- a/report/BoSung/BoSungNoiDung.xlsx
+++ b/report/BoSung/BoSungNoiDung.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Từ viết tắt" sheetId="1" r:id="rId1"/>
     <sheet name="Diễn nghĩa thuật ngữ" sheetId="2" r:id="rId2"/>
+    <sheet name="Diễn nghĩa khái niệm" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>STT</t>
   </si>
@@ -63,6 +64,27 @@
   </si>
   <si>
     <t>plug-in</t>
+  </si>
+  <si>
+    <t>Khái niệm</t>
+  </si>
+  <si>
+    <t>Eclipse</t>
+  </si>
+  <si>
+    <t>SDK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smartphone </t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>JDK</t>
+  </si>
+  <si>
+    <t>API</t>
   </si>
 </sst>
 </file>
@@ -113,7 +135,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -153,10 +187,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B9" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:B11"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Thuật ngữ" dataDxfId="1"/>
+    <tableColumn id="1" name="Thuật ngữ" dataDxfId="5"/>
+    <tableColumn id="2" name="Diễn nghĩa" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table33" displayName="Table33" ref="A1:B10" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B10"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Khái niệm" dataDxfId="1"/>
     <tableColumn id="2" name="Diễn nghĩa" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -452,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,15 +543,24 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -564,10 +618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +688,18 @@
       </c>
       <c r="B9" s="3"/>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -641,4 +707,72 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="80.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>